<commit_message>
- added some grades
</commit_message>
<xml_diff>
--- a/Resources/30434.xlsx
+++ b/Resources/30434.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Predare\2017-2018 - sem 2\SoftwareDesign2017\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{81143EE6-620E-4D30-8235-3766E2DFEF4A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="1" r:id="rId1"/>
@@ -230,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,7 +522,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -857,7 +858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
@@ -30510,11 +30511,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30644,15 +30645,19 @@
       <c r="E3" s="1">
         <v>10</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="1">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="6">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="M3" s="6">
         <f t="shared" si="2"/>
@@ -30683,15 +30688,19 @@
       <c r="E4" s="4">
         <v>10</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="4">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4">
+        <v>10</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="M4" s="4">
         <f t="shared" si="2"/>
@@ -30761,15 +30770,19 @@
       <c r="E6" s="4">
         <v>10</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="4">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4">
+        <v>10</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" si="2"/>
@@ -30798,9 +30811,11 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="F7" s="1">
+        <v>12</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -30808,7 +30823,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="6">
         <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
+        <v>7</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
@@ -30839,15 +30854,19 @@
       <c r="E8" s="4">
         <v>10</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="4">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4">
+        <v>10</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="2"/>
@@ -30878,15 +30897,19 @@
       <c r="E9" s="1">
         <v>10</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="F9" s="1">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="6">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="2"/>
@@ -30956,15 +30979,19 @@
       <c r="E11" s="1">
         <v>10</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="1">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="6">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" si="2"/>
@@ -30995,7 +31022,9 @@
       <c r="E12" s="17">
         <v>5</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4">
+        <v>9</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -31003,7 +31032,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="2"/>
@@ -31034,15 +31063,19 @@
       <c r="E13" s="1">
         <v>10</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="F13" s="1">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1">
+        <v>10</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="6">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="M13" s="6">
         <f t="shared" si="2"/>
@@ -31188,17 +31221,21 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="F17" s="1">
+        <v>14</v>
+      </c>
+      <c r="G17" s="1">
+        <v>10</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="6">
         <f t="shared" si="1"/>
-        <v>2.1666666666666665</v>
+        <v>11</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" si="2"/>
@@ -31229,15 +31266,19 @@
       <c r="E18" s="4">
         <v>9</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="4">
+        <v>11</v>
+      </c>
+      <c r="G18" s="4">
+        <v>10</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M18" s="4">
         <f t="shared" si="2"/>
@@ -31270,15 +31311,19 @@
       <c r="E19" s="1">
         <v>10</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="F19" s="1">
+        <v>14</v>
+      </c>
+      <c r="G19" s="1">
+        <v>10</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="6">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="2"/>
@@ -31309,15 +31354,19 @@
       <c r="E20" s="4">
         <v>9</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="F20" s="4">
+        <v>14</v>
+      </c>
+      <c r="G20" s="4">
+        <v>10</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M20" s="4">
         <f t="shared" si="2"/>
@@ -31348,15 +31397,19 @@
       <c r="E21" s="1">
         <v>10</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="F21" s="1">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1">
+        <v>10</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="6">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="M21" s="6">
         <f t="shared" si="2"/>
@@ -31385,17 +31438,19 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4">
+        <v>10</v>
+      </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>5</v>
       </c>
       <c r="M22" s="4">
         <f t="shared" si="2"/>
@@ -31426,15 +31481,19 @@
       <c r="E23" s="1">
         <v>9</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="1">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1">
+        <v>10</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M23" s="6">
         <f t="shared" si="2"/>
@@ -31467,15 +31526,19 @@
       <c r="E24" s="4">
         <v>9</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="4">
+        <v>12</v>
+      </c>
+      <c r="G24" s="4">
+        <v>10</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>10.333333333333334</v>
       </c>
       <c r="M24" s="4">
         <f t="shared" si="2"/>
@@ -31506,15 +31569,19 @@
       <c r="E25" s="1">
         <v>10</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1">
+        <v>14</v>
+      </c>
+      <c r="G25" s="1">
+        <v>10</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="6">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="M25" s="6">
         <f t="shared" si="2"/>
@@ -31545,15 +31612,19 @@
       <c r="E26" s="4">
         <v>10</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="F26" s="4">
+        <v>14</v>
+      </c>
+      <c r="G26" s="4">
+        <v>10</v>
+      </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="M26" s="4">
         <f t="shared" si="2"/>
@@ -31701,7 +31772,9 @@
       <c r="E30" s="4">
         <v>1</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="4">
+        <v>11</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -31709,7 +31782,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4">
         <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
+        <v>4</v>
       </c>
       <c r="M30" s="4">
         <f t="shared" si="4"/>
@@ -31931,15 +32004,19 @@
       <c r="E36" s="4">
         <v>10</v>
       </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="F36" s="4">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4">
+        <v>10</v>
+      </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4">
         <f t="shared" si="5"/>
-        <v>3.3333333333333335</v>
+        <v>10.666666666666666</v>
       </c>
       <c r="M36" s="4">
         <f t="shared" si="6"/>
@@ -31970,7 +32047,9 @@
       <c r="E37" s="6">
         <v>8</v>
       </c>
-      <c r="F37" s="6"/>
+      <c r="F37" s="6">
+        <v>5</v>
+      </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -31978,7 +32057,7 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6">
         <f t="shared" si="5"/>
-        <v>2.6666666666666665</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="M37" s="6">
         <f t="shared" si="6"/>
@@ -57040,7 +57119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
[ACC] - some grading
</commit_message>
<xml_diff>
--- a/Resources/30434.xlsx
+++ b/Resources/30434.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>Facultatea -</t>
   </si>
@@ -88,10 +88,16 @@
     <t>Lab 14</t>
   </si>
   <si>
+    <t>Extra p</t>
+  </si>
+  <si>
     <t>Baias Ioan Nicolae</t>
   </si>
   <si>
     <t>Balas Andrei Ioan</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
   <si>
     <t>Baraian Tudor-Stefan</t>
@@ -578,7 +584,7 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -2181,7 +2187,7 @@
       <c r="W11" s="11"/>
       <c r="X11" s="11"/>
       <c r="Y11" s="11"/>
-      <c r="Z11" s="7"/>
+      <c r="Z11" s="11"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="9"/>
     </row>
@@ -2247,8 +2253,10 @@
       <c r="Y12" t="s" s="22">
         <v>24</v>
       </c>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="7"/>
+      <c r="Z12" t="s" s="22">
+        <v>25</v>
+      </c>
+      <c r="AA12" s="23"/>
       <c r="AB12" s="9"/>
     </row>
     <row r="13" ht="13.7" customHeight="1">
@@ -2260,7 +2268,7 @@
       </c>
       <c r="E13" s="26"/>
       <c r="F13" t="s" s="27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
@@ -2283,8 +2291,8 @@
       <c r="W13" s="26"/>
       <c r="X13" s="26"/>
       <c r="Y13" s="26"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="7"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="23"/>
       <c r="AB13" s="9"/>
     </row>
     <row r="14" ht="13.7" customHeight="1">
@@ -2296,7 +2304,7 @@
       </c>
       <c r="E14" s="26"/>
       <c r="F14" t="s" s="27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
@@ -2321,8 +2329,10 @@
       <c r="W14" s="26"/>
       <c r="X14" s="26"/>
       <c r="Y14" s="26"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="7"/>
+      <c r="Z14" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA14" s="23"/>
       <c r="AB14" s="9"/>
     </row>
     <row r="15" ht="13.7" customHeight="1">
@@ -2334,7 +2344,7 @@
       </c>
       <c r="E15" s="26"/>
       <c r="F15" t="s" s="27">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
@@ -2359,8 +2369,8 @@
       <c r="W15" s="26"/>
       <c r="X15" s="26"/>
       <c r="Y15" s="26"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="7"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="23"/>
       <c r="AB15" s="9"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
@@ -2372,7 +2382,7 @@
       </c>
       <c r="E16" s="26"/>
       <c r="F16" t="s" s="27">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
@@ -2397,8 +2407,10 @@
       <c r="W16" s="26"/>
       <c r="X16" s="26"/>
       <c r="Y16" s="26"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="7"/>
+      <c r="Z16" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA16" s="23"/>
       <c r="AB16" s="9"/>
     </row>
     <row r="17" ht="13.7" customHeight="1">
@@ -2410,7 +2422,7 @@
       </c>
       <c r="E17" s="26"/>
       <c r="F17" t="s" s="27">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
@@ -2435,8 +2447,8 @@
       <c r="W17" s="26"/>
       <c r="X17" s="26"/>
       <c r="Y17" s="26"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="7"/>
+      <c r="Z17" s="26"/>
+      <c r="AA17" s="23"/>
       <c r="AB17" s="9"/>
     </row>
     <row r="18" ht="13.7" customHeight="1">
@@ -2448,7 +2460,7 @@
       </c>
       <c r="E18" s="26"/>
       <c r="F18" t="s" s="27">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
@@ -2463,7 +2475,7 @@
       <c r="Q18" s="26"/>
       <c r="R18" s="26"/>
       <c r="S18" t="s" s="30">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T18" s="26"/>
       <c r="U18" s="26"/>
@@ -2471,8 +2483,8 @@
       <c r="W18" s="26"/>
       <c r="X18" s="26"/>
       <c r="Y18" s="26"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="7"/>
+      <c r="Z18" s="26"/>
+      <c r="AA18" s="23"/>
       <c r="AB18" s="9"/>
     </row>
     <row r="19" ht="13.7" customHeight="1">
@@ -2484,7 +2496,7 @@
       </c>
       <c r="E19" s="26"/>
       <c r="F19" t="s" s="27">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -2501,7 +2513,7 @@
       <c r="Q19" s="26"/>
       <c r="R19" s="26"/>
       <c r="S19" t="s" s="30">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T19" s="26"/>
       <c r="U19" s="26"/>
@@ -2509,8 +2521,10 @@
       <c r="W19" s="26"/>
       <c r="X19" s="26"/>
       <c r="Y19" s="26"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="7"/>
+      <c r="Z19" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA19" s="23"/>
       <c r="AB19" s="9"/>
     </row>
     <row r="20" ht="13.7" customHeight="1">
@@ -2522,7 +2536,7 @@
       </c>
       <c r="E20" s="26"/>
       <c r="F20" t="s" s="27">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
@@ -2547,8 +2561,10 @@
       <c r="W20" s="26"/>
       <c r="X20" s="26"/>
       <c r="Y20" s="26"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="7"/>
+      <c r="Z20" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA20" s="23"/>
       <c r="AB20" s="9"/>
     </row>
     <row r="21" ht="13.7" customHeight="1">
@@ -2560,7 +2576,7 @@
       </c>
       <c r="E21" s="26"/>
       <c r="F21" t="s" s="27">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
@@ -2585,8 +2601,10 @@
       <c r="W21" s="26"/>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="7"/>
+      <c r="Z21" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA21" s="23"/>
       <c r="AB21" s="9"/>
     </row>
     <row r="22" ht="13.7" customHeight="1">
@@ -2598,7 +2616,7 @@
       </c>
       <c r="E22" s="26"/>
       <c r="F22" t="s" s="27">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -2619,8 +2637,8 @@
       <c r="W22" s="26"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
-      <c r="Z22" s="23"/>
-      <c r="AA22" s="7"/>
+      <c r="Z22" s="26"/>
+      <c r="AA22" s="23"/>
       <c r="AB22" s="9"/>
     </row>
     <row r="23" ht="13.7" customHeight="1">
@@ -2632,7 +2650,7 @@
       </c>
       <c r="E23" s="26"/>
       <c r="F23" t="s" s="27">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
@@ -2653,8 +2671,8 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26"/>
-      <c r="Z23" s="23"/>
-      <c r="AA23" s="7"/>
+      <c r="Z23" s="26"/>
+      <c r="AA23" s="23"/>
       <c r="AB23" s="9"/>
     </row>
     <row r="24" ht="13.7" customHeight="1">
@@ -2666,7 +2684,7 @@
       </c>
       <c r="E24" s="26"/>
       <c r="F24" t="s" s="27">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
@@ -2691,8 +2709,10 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26"/>
-      <c r="Z24" s="23"/>
-      <c r="AA24" s="7"/>
+      <c r="Z24" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA24" s="23"/>
       <c r="AB24" s="9"/>
     </row>
     <row r="25" ht="13.7" customHeight="1">
@@ -2704,7 +2724,7 @@
       </c>
       <c r="E25" s="26"/>
       <c r="F25" t="s" s="27">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
@@ -2727,8 +2747,8 @@
       <c r="W25" s="26"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
-      <c r="Z25" s="23"/>
-      <c r="AA25" s="7"/>
+      <c r="Z25" s="26"/>
+      <c r="AA25" s="23"/>
       <c r="AB25" s="9"/>
     </row>
     <row r="26" ht="13.7" customHeight="1">
@@ -2740,7 +2760,7 @@
       </c>
       <c r="E26" s="26"/>
       <c r="F26" t="s" s="27">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
@@ -2765,8 +2785,8 @@
       <c r="W26" s="26"/>
       <c r="X26" s="26"/>
       <c r="Y26" s="26"/>
-      <c r="Z26" s="23"/>
-      <c r="AA26" s="7"/>
+      <c r="Z26" s="26"/>
+      <c r="AA26" s="23"/>
       <c r="AB26" s="9"/>
     </row>
     <row r="27" ht="13.7" customHeight="1">
@@ -2778,7 +2798,7 @@
       </c>
       <c r="E27" s="26"/>
       <c r="F27" t="s" s="27">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
@@ -2803,8 +2823,10 @@
       <c r="W27" s="26"/>
       <c r="X27" s="26"/>
       <c r="Y27" s="26"/>
-      <c r="Z27" s="23"/>
-      <c r="AA27" s="7"/>
+      <c r="Z27" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA27" s="23"/>
       <c r="AB27" s="9"/>
     </row>
     <row r="28" ht="13.7" customHeight="1">
@@ -2816,7 +2838,7 @@
       </c>
       <c r="E28" s="26"/>
       <c r="F28" t="s" s="27">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
@@ -2839,8 +2861,8 @@
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
-      <c r="Z28" s="23"/>
-      <c r="AA28" s="7"/>
+      <c r="Z28" s="26"/>
+      <c r="AA28" s="23"/>
       <c r="AB28" s="9"/>
     </row>
     <row r="29" ht="13.7" customHeight="1">
@@ -2852,7 +2874,7 @@
       </c>
       <c r="E29" s="26"/>
       <c r="F29" t="s" s="27">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
@@ -2869,7 +2891,7 @@
       <c r="Q29" s="26"/>
       <c r="R29" s="26"/>
       <c r="S29" t="s" s="30">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T29" s="26"/>
       <c r="U29" s="26"/>
@@ -2877,8 +2899,8 @@
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
       <c r="Y29" s="26"/>
-      <c r="Z29" s="23"/>
-      <c r="AA29" s="7"/>
+      <c r="Z29" s="26"/>
+      <c r="AA29" s="23"/>
       <c r="AB29" s="9"/>
     </row>
     <row r="30" ht="13.7" customHeight="1">
@@ -2890,7 +2912,7 @@
       </c>
       <c r="E30" s="26"/>
       <c r="F30" t="s" s="27">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
@@ -2915,8 +2937,8 @@
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
-      <c r="Z30" s="23"/>
-      <c r="AA30" s="7"/>
+      <c r="Z30" s="26"/>
+      <c r="AA30" s="23"/>
       <c r="AB30" s="9"/>
     </row>
     <row r="31" ht="13.7" customHeight="1">
@@ -2928,7 +2950,7 @@
       </c>
       <c r="E31" s="26"/>
       <c r="F31" t="s" s="27">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
@@ -2949,8 +2971,8 @@
       <c r="W31" s="26"/>
       <c r="X31" s="26"/>
       <c r="Y31" s="26"/>
-      <c r="Z31" s="23"/>
-      <c r="AA31" s="7"/>
+      <c r="Z31" s="26"/>
+      <c r="AA31" s="23"/>
       <c r="AB31" s="9"/>
     </row>
     <row r="32" ht="13.7" customHeight="1">
@@ -2962,7 +2984,7 @@
       </c>
       <c r="E32" s="26"/>
       <c r="F32" t="s" s="27">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
@@ -2985,8 +3007,10 @@
       <c r="W32" s="26"/>
       <c r="X32" s="26"/>
       <c r="Y32" s="26"/>
-      <c r="Z32" s="23"/>
-      <c r="AA32" s="7"/>
+      <c r="Z32" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA32" s="23"/>
       <c r="AB32" s="9"/>
     </row>
     <row r="33" ht="13.7" customHeight="1">
@@ -2998,7 +3022,7 @@
       </c>
       <c r="E33" s="26"/>
       <c r="F33" t="s" s="27">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
@@ -3047,8 +3071,8 @@
       <c r="Y33" s="29">
         <v>5</v>
       </c>
-      <c r="Z33" s="23"/>
-      <c r="AA33" s="7"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="23"/>
       <c r="AB33" s="9"/>
     </row>
     <row r="34" ht="13.7" customHeight="1">
@@ -3060,7 +3084,7 @@
       </c>
       <c r="E34" s="26"/>
       <c r="F34" t="s" s="27">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
@@ -3109,8 +3133,8 @@
       <c r="Y34" s="29">
         <v>5</v>
       </c>
-      <c r="Z34" s="23"/>
-      <c r="AA34" s="7"/>
+      <c r="Z34" s="26"/>
+      <c r="AA34" s="23"/>
       <c r="AB34" s="9"/>
     </row>
     <row r="35" ht="13.7" customHeight="1">
@@ -3122,7 +3146,7 @@
       </c>
       <c r="E35" s="26"/>
       <c r="F35" t="s" s="27">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
@@ -3147,8 +3171,8 @@
       <c r="W35" s="26"/>
       <c r="X35" s="26"/>
       <c r="Y35" s="26"/>
-      <c r="Z35" s="23"/>
-      <c r="AA35" s="7"/>
+      <c r="Z35" s="26"/>
+      <c r="AA35" s="23"/>
       <c r="AB35" s="9"/>
     </row>
     <row r="36" ht="13.7" customHeight="1">
@@ -3160,7 +3184,7 @@
       </c>
       <c r="E36" s="26"/>
       <c r="F36" t="s" s="27">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
@@ -3183,8 +3207,10 @@
       <c r="W36" s="26"/>
       <c r="X36" s="26"/>
       <c r="Y36" s="26"/>
-      <c r="Z36" s="23"/>
-      <c r="AA36" s="7"/>
+      <c r="Z36" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA36" s="23"/>
       <c r="AB36" s="9"/>
     </row>
     <row r="37" ht="13.7" customHeight="1">
@@ -3196,7 +3222,7 @@
       </c>
       <c r="E37" s="26"/>
       <c r="F37" t="s" s="27">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
@@ -3221,8 +3247,8 @@
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
       <c r="Y37" s="26"/>
-      <c r="Z37" s="23"/>
-      <c r="AA37" s="7"/>
+      <c r="Z37" s="26"/>
+      <c r="AA37" s="23"/>
       <c r="AB37" s="9"/>
     </row>
     <row r="38" ht="13.7" customHeight="1">
@@ -3234,7 +3260,7 @@
       </c>
       <c r="E38" s="26"/>
       <c r="F38" t="s" s="27">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
@@ -3257,8 +3283,8 @@
       <c r="W38" s="26"/>
       <c r="X38" s="26"/>
       <c r="Y38" s="26"/>
-      <c r="Z38" s="23"/>
-      <c r="AA38" s="7"/>
+      <c r="Z38" s="26"/>
+      <c r="AA38" s="23"/>
       <c r="AB38" s="9"/>
     </row>
     <row r="39" ht="13.7" customHeight="1">
@@ -3270,7 +3296,7 @@
       </c>
       <c r="E39" s="26"/>
       <c r="F39" t="s" s="27">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
@@ -3287,7 +3313,7 @@
       <c r="Q39" s="26"/>
       <c r="R39" s="26"/>
       <c r="S39" t="s" s="30">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="T39" s="26"/>
       <c r="U39" s="26"/>
@@ -3295,8 +3321,8 @@
       <c r="W39" s="26"/>
       <c r="X39" s="26"/>
       <c r="Y39" s="26"/>
-      <c r="Z39" s="23"/>
-      <c r="AA39" s="7"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="23"/>
       <c r="AB39" s="9"/>
     </row>
     <row r="40" ht="13.7" customHeight="1">
@@ -3308,7 +3334,7 @@
       </c>
       <c r="E40" s="26"/>
       <c r="F40" t="s" s="27">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
@@ -3333,8 +3359,8 @@
       <c r="W40" s="26"/>
       <c r="X40" s="26"/>
       <c r="Y40" s="26"/>
-      <c r="Z40" s="23"/>
-      <c r="AA40" s="7"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="23"/>
       <c r="AB40" s="9"/>
     </row>
     <row r="41" ht="13.7" customHeight="1">
@@ -3346,7 +3372,7 @@
       </c>
       <c r="E41" s="26"/>
       <c r="F41" t="s" s="27">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
@@ -3367,8 +3393,10 @@
       <c r="W41" s="26"/>
       <c r="X41" s="26"/>
       <c r="Y41" s="26"/>
-      <c r="Z41" s="23"/>
-      <c r="AA41" s="7"/>
+      <c r="Z41" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="AA41" s="23"/>
       <c r="AB41" s="9"/>
     </row>
     <row r="42" ht="13.7" customHeight="1">
@@ -3380,7 +3408,7 @@
       </c>
       <c r="E42" s="26"/>
       <c r="F42" t="s" s="27">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
@@ -3397,7 +3425,7 @@
       <c r="Q42" s="26"/>
       <c r="R42" s="26"/>
       <c r="S42" t="s" s="30">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="T42" s="26"/>
       <c r="U42" s="26"/>
@@ -3405,8 +3433,8 @@
       <c r="W42" s="26"/>
       <c r="X42" s="26"/>
       <c r="Y42" s="26"/>
-      <c r="Z42" s="35"/>
-      <c r="AA42" s="32"/>
+      <c r="Z42" s="26"/>
+      <c r="AA42" s="35"/>
       <c r="AB42" s="36"/>
     </row>
     <row r="43" ht="13.7" customHeight="1">

</xml_diff>